<commit_message>
revise the can protocol
</commit_message>
<xml_diff>
--- a/Doc/Protocol/CAN总线协议.xlsx
+++ b/Doc/Protocol/CAN总线协议.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F1A068-9D90-43AB-A2C9-934310CC8F67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81280C30-A3ED-4B92-8A4E-40C4AA777ACB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="超声波原始数据(RX)" sheetId="12" r:id="rId1"/>
@@ -16,9 +16,9 @@
     <sheet name="车速反馈(RX)" sheetId="4" r:id="rId6"/>
     <sheet name="车速注入(TX)" sheetId="15" r:id="rId7"/>
     <sheet name="系统状态反馈(RX)" sheetId="9" r:id="rId8"/>
-    <sheet name="系统工作模式配置(TX)" sheetId="7" r:id="rId9"/>
-    <sheet name="车辆跟踪信息(RX)" sheetId="18" r:id="rId10"/>
-    <sheet name="车位信息(TX)" sheetId="19" r:id="rId11"/>
+    <sheet name="车位信息(TX)" sheetId="19" r:id="rId9"/>
+    <sheet name="系统工作模式配置(TX)" sheetId="7" r:id="rId10"/>
+    <sheet name="车辆跟踪信息(RX)" sheetId="18" r:id="rId11"/>
     <sheet name="应答信号(RX)" sheetId="14" r:id="rId12"/>
     <sheet name="PID调试帧(TX)" sheetId="5" r:id="rId13"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="215">
   <si>
     <t>字节</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -863,6 +863,18 @@
   </si>
   <si>
     <t>[0;0x5A]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1457,46 +1469,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="10" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="11" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="11" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="8" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="9" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2049,1051 +2061,624 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035C941A-BCE1-46E3-89DE-EEDC1055935D}">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8238FD7-9016-4AA5-B4BA-2804821B8803}">
+  <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="5.9140625" customWidth="1"/>
+    <col min="9" max="9" width="8.58203125" customWidth="1"/>
+    <col min="10" max="10" width="6.08203125" customWidth="1"/>
+    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="12" max="12" width="7.75" customWidth="1"/>
+    <col min="18" max="18" width="16.83203125" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="30" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+    </row>
+    <row r="3" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E3" s="75">
         <v>8</v>
       </c>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="49">
+      <c r="F3" s="76"/>
+    </row>
+    <row r="4" spans="1:22" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="49">
-        <v>1</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="49">
+      <c r="B4" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="48">
+        <v>1</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="48">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>200</v>
+      </c>
+      <c r="I4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E5" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="49">
+      <c r="B6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="49">
+      <c r="B7" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="49">
+      <c r="B8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
+      <c r="B9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="49">
+      <c r="B10" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="30" t="s">
+      <c r="B11" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="76"/>
+      <c r="D12" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="75">
         <v>8</v>
       </c>
-      <c r="F12" s="53"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="52">
+      <c r="F12" s="76"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="74"/>
+    </row>
+    <row r="13" spans="1:22" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>0</v>
       </c>
-      <c r="B13" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="55">
-        <v>1E-3</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="52">
-        <v>1</v>
-      </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52">
+      <c r="B13" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="27">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="74">
+        <v>0</v>
+      </c>
+      <c r="I13" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="38">
+        <v>1</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="38">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="55" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="55">
-        <v>1E-3</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="52">
+      <c r="B15" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="4">
+        <v>2</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="52">
+      <c r="B16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="74">
+        <v>1</v>
+      </c>
+      <c r="I16" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>4</v>
       </c>
-      <c r="B17" s="55" t="s">
-        <v>182</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="55">
-        <v>1E-3</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="52">
+      <c r="B17" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="52">
+      <c r="B18" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>6</v>
       </c>
-      <c r="B19" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="55">
-        <v>1E-3</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="52">
+      <c r="B19" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="74">
+        <v>2</v>
+      </c>
+      <c r="I19" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>7</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-    </row>
-    <row r="21" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="63" t="s">
-        <v>189</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="B20" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="4">
+        <v>2</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="11"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="4">
+        <v>3</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G23" s="6"/>
+      <c r="H23" s="74">
+        <v>3</v>
+      </c>
+      <c r="I23" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="4">
         <v>0</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="53" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="53">
-        <v>8</v>
-      </c>
-      <c r="F23" s="53"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="46">
-        <v>0</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F24" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="46">
-        <v>1</v>
-      </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="46">
+      <c r="K23" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G24" s="6"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="4">
+        <v>1</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="4">
         <v>2</v>
       </c>
-      <c r="B26" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="46">
+      <c r="K25" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="6"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="4">
         <v>3</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="46">
+      <c r="K26" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G27" s="6"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="4">
         <v>4</v>
       </c>
-      <c r="B28" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F28" s="55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="46">
-        <v>5</v>
-      </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="46">
-        <v>6</v>
-      </c>
-      <c r="B30" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="55" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="46">
-        <v>7</v>
-      </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-    </row>
-    <row r="32" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="63" t="s">
-        <v>188</v>
-      </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="53">
-        <v>8</v>
-      </c>
-      <c r="F33" s="53"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="49">
-        <v>0</v>
-      </c>
-      <c r="B34" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E34" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F34" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="49">
-        <v>1</v>
-      </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="49">
-        <v>2</v>
-      </c>
-      <c r="B36" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C36" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E36" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F36" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="49">
-        <v>3</v>
-      </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="49">
-        <v>4</v>
-      </c>
-      <c r="B38" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C38" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E38" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F38" s="55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="49">
-        <v>5</v>
-      </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="49">
-        <v>6</v>
-      </c>
-      <c r="B40" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="C40" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="48">
-        <v>1</v>
-      </c>
-      <c r="E40" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="F40" s="48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="49">
-        <v>7</v>
-      </c>
-      <c r="B41" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="63" t="s">
-        <v>190</v>
-      </c>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>207</v>
-      </c>
-      <c r="C43" s="53"/>
-      <c r="D43" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" s="53">
-        <v>8</v>
-      </c>
-      <c r="F43" s="53"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="49">
-        <v>0</v>
-      </c>
-      <c r="B44" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E44" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F44" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="49">
-        <v>1</v>
-      </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="49">
-        <v>2</v>
-      </c>
-      <c r="B46" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E46" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F46" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="49">
-        <v>3</v>
-      </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="49">
-        <v>4</v>
-      </c>
-      <c r="B48" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C48" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E48" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F48" s="55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="49">
-        <v>5</v>
-      </c>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="49">
-        <v>6</v>
-      </c>
-      <c r="B50" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="D50" s="48">
-        <v>1</v>
-      </c>
-      <c r="E50" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="F50" s="48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="49">
-        <v>7</v>
-      </c>
-      <c r="B51" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="63" t="s">
-        <v>208</v>
-      </c>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="53">
-        <v>8</v>
-      </c>
-      <c r="F53" s="53"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="52">
-        <v>0</v>
-      </c>
-      <c r="B54" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C54" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E54" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F54" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="52">
-        <v>1</v>
-      </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="52">
-        <v>2</v>
-      </c>
-      <c r="B56" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C56" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E56" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F56" s="55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="52">
-        <v>3</v>
-      </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="52">
-        <v>4</v>
-      </c>
-      <c r="B58" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C58" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E58" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F58" s="55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="52">
-        <v>5</v>
-      </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="52">
-        <v>6</v>
-      </c>
-      <c r="B60" s="51" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="51">
-        <v>1</v>
-      </c>
-      <c r="E60" s="51" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="52">
-        <v>7</v>
-      </c>
-      <c r="B61" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D61" s="51">
-        <v>1</v>
-      </c>
-      <c r="E61" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="F61" s="51" t="s">
-        <v>18</v>
+      <c r="K27" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="118">
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A11:F11"/>
+  <mergeCells count="15">
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3102,51 +2687,51 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3B3C39-6194-4D88-96DE-4A9D4173FD26}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035C941A-BCE1-46E3-89DE-EEDC1055935D}">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F20" sqref="A12:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C3" s="53"/>
       <c r="D3" s="30" t="s">
@@ -3251,48 +2836,48 @@
       <c r="A10" s="49">
         <v>6</v>
       </c>
-      <c r="B10" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="55">
-        <v>0.01</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" s="55" t="s">
-        <v>172</v>
+      <c r="B10" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="52">
+        <v>1</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="F10" s="52">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="49">
         <v>7</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="30" t="s">
@@ -3304,7 +2889,7 @@
       <c r="F13" s="53"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="49">
+      <c r="A14" s="51">
         <v>0</v>
       </c>
       <c r="B14" s="55" t="s">
@@ -3324,7 +2909,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
+      <c r="A15" s="51">
         <v>1</v>
       </c>
       <c r="B15" s="55"/>
@@ -3334,7 +2919,7 @@
       <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="49">
+      <c r="A16" s="51">
         <v>2</v>
       </c>
       <c r="B16" s="55" t="s">
@@ -3354,7 +2939,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="49">
+      <c r="A17" s="51">
         <v>3</v>
       </c>
       <c r="B17" s="55"/>
@@ -3364,7 +2949,7 @@
       <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="49">
+      <c r="A18" s="51">
         <v>4</v>
       </c>
       <c r="B18" s="55" t="s">
@@ -3384,7 +2969,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
+      <c r="A19" s="51">
         <v>5</v>
       </c>
       <c r="B19" s="55"/>
@@ -3394,7 +2979,7 @@
       <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="49">
+      <c r="A20" s="51">
         <v>6</v>
       </c>
       <c r="B20" s="55" t="s">
@@ -3414,7 +2999,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="49">
+      <c r="A21" s="51">
         <v>7</v>
       </c>
       <c r="B21" s="55"/>
@@ -3423,47 +3008,705 @@
       <c r="E21" s="55"/>
       <c r="F21" s="55"/>
     </row>
+    <row r="22" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="53"/>
+      <c r="D24" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="53">
+        <v>8</v>
+      </c>
+      <c r="F24" s="53"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="46">
+        <v>0</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="46">
+        <v>1</v>
+      </c>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="46">
+        <v>2</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="46">
+        <v>3</v>
+      </c>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="46">
+        <v>4</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="46">
+        <v>5</v>
+      </c>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="46">
+        <v>6</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="46">
+        <v>7</v>
+      </c>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+    </row>
+    <row r="33" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="53"/>
+      <c r="D34" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="53">
+        <v>8</v>
+      </c>
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="49">
+        <v>0</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="49">
+        <v>1</v>
+      </c>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="49">
+        <v>2</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="49">
+        <v>3</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="49">
+        <v>4</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E39" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="49">
+        <v>5</v>
+      </c>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="49">
+        <v>6</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="48">
+        <v>1</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="49">
+        <v>7</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="53"/>
+      <c r="D44" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="53">
+        <v>8</v>
+      </c>
+      <c r="F44" s="53"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="49">
+        <v>0</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E45" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="49">
+        <v>1</v>
+      </c>
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="49">
+        <v>2</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F47" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="49">
+        <v>3</v>
+      </c>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="49">
+        <v>4</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E49" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F49" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="49">
+        <v>5</v>
+      </c>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="49">
+        <v>6</v>
+      </c>
+      <c r="B51" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="D51" s="48">
+        <v>1</v>
+      </c>
+      <c r="E51" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="F51" s="48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="49">
+        <v>7</v>
+      </c>
+      <c r="B52" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="C54" s="53"/>
+      <c r="D54" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" s="53">
+        <v>8</v>
+      </c>
+      <c r="F54" s="53"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="51">
+        <v>0</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E55" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F55" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="51">
+        <v>1</v>
+      </c>
+      <c r="B56" s="55"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="51">
+        <v>2</v>
+      </c>
+      <c r="B57" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E57" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F57" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="51">
+        <v>3</v>
+      </c>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="51">
+        <v>4</v>
+      </c>
+      <c r="B59" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E59" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F59" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="51">
+        <v>5</v>
+      </c>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="51">
+        <v>6</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" s="50">
+        <v>1</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="F61" s="50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="51">
+        <v>7</v>
+      </c>
+      <c r="B62" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="50">
+        <v>1</v>
+      </c>
+      <c r="E62" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="F62" s="50" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B13:C13"/>
+  <mergeCells count="118">
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B4:B5"/>
@@ -3471,6 +3714,54 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3489,14 +3780,14 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -3720,14 +4011,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -4377,14 +4668,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -4421,19 +4712,19 @@
         <v>8</v>
       </c>
       <c r="F3" s="53"/>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="61"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="59">
+      <c r="A4" s="63">
         <v>0</v>
       </c>
       <c r="B4" s="55" t="s">
@@ -4477,7 +4768,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
@@ -4925,6 +5216,8 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="G3:N3"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="F19:F20"/>
@@ -4940,9 +5233,7 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A4:A5"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C4:C5"/>
@@ -4981,14 +5272,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -5027,7 +5318,7 @@
       <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="59">
+      <c r="A4" s="63">
         <v>0</v>
       </c>
       <c r="B4" s="55" t="s">
@@ -5047,7 +5338,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
@@ -5214,14 +5505,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -5788,14 +6079,14 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -6174,14 +6465,14 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -6387,14 +6678,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
       <c r="G1" s="6"/>
       <c r="H1" s="74" t="s">
         <v>66</v>
@@ -6785,624 +7076,375 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8238FD7-9016-4AA5-B4BA-2804821B8803}">
-  <dimension ref="A1:V27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3B3C39-6194-4D88-96DE-4A9D4173FD26}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J5"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="8" width="5.9140625" customWidth="1"/>
-    <col min="9" max="9" width="8.58203125" customWidth="1"/>
-    <col min="10" max="10" width="6.08203125" customWidth="1"/>
-    <col min="11" max="11" width="16.75" customWidth="1"/>
-    <col min="12" max="12" width="7.75" customWidth="1"/>
-    <col min="18" max="18" width="16.83203125" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="32" t="s">
+    <row r="2" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="53">
         <v>8</v>
       </c>
-      <c r="F3" s="76"/>
-    </row>
-    <row r="4" spans="1:22" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="49">
         <v>0</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="48">
-        <v>1</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="48">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>200</v>
-      </c>
-      <c r="I4" t="s">
-        <v>201</v>
-      </c>
-      <c r="J4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>1</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>202</v>
-      </c>
-      <c r="J5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="B4" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="49">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="49">
         <v>2</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="B6" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="49">
         <v>3</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="49">
         <v>4</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="B8" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="49">
         <v>5</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="49">
         <v>6</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="B10" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="49">
         <v>7</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="32" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="75">
+      <c r="E13" s="53">
         <v>8</v>
       </c>
-      <c r="F12" s="76"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="74"/>
-    </row>
-    <row r="13" spans="1:22" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="F13" s="53"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="49">
         <v>0</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="27">
-        <v>1</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="27">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="74">
-        <v>0</v>
-      </c>
-      <c r="I13" s="74" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>1</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="38">
-        <v>1</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="F14" s="38">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="4">
-        <v>1</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="B14" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="49">
+        <v>1</v>
+      </c>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="49">
         <v>2</v>
       </c>
-      <c r="B15" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="4">
-        <v>2</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="B16" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="49">
         <v>3</v>
       </c>
-      <c r="B16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="74">
-        <v>1</v>
-      </c>
-      <c r="I16" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="49">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="4">
-        <v>1</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="B18" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="49">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="3">
-        <v>2</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="49">
         <v>6</v>
       </c>
-      <c r="B19" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="74">
-        <v>2</v>
-      </c>
-      <c r="I19" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="B20" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="49">
         <v>7</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="4">
-        <v>1</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="4">
-        <v>2</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G22" s="11"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="4">
-        <v>3</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G23" s="6"/>
-      <c r="H23" s="74">
-        <v>3</v>
-      </c>
-      <c r="I23" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G24" s="6"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="4">
-        <v>1</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G25" s="6"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="4">
-        <v>2</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G26" s="6"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="4">
-        <v>3</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G27" s="6"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="4">
-        <v>4</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="H19:H22"/>
+  <mergeCells count="46">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>